<commit_message>
complete data from ST
</commit_message>
<xml_diff>
--- a/data/msrtc/data/data/latlong/solapur.xlsx
+++ b/data/msrtc/data/data/latlong/solapur.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7896" uniqueCount="4064">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7894" uniqueCount="4064">
   <si>
     <t>Aurangabad</t>
   </si>
@@ -13501,7 +13501,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
+      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14707,11 +14707,11 @@
       <c r="D38" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>520</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>521</v>
+      <c r="E38" s="9">
+        <v>17.48094</v>
+      </c>
+      <c r="F38" s="9">
+        <v>76.110111000000003</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>4035</v>

</xml_diff>